<commit_message>
Test suite updates 4/23 **changed order of test suite tests; this should address some product issues identified **other minor changes
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/backdatedVinTable_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/backdatedVinTable_UT_SS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT-repo\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Documents\CSAA\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9732"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -231,31 +231,31 @@
     <t>BACKDATED_SS</t>
   </si>
   <si>
+    <t>7MSRP15H&amp;V</t>
+  </si>
+  <si>
+    <t>VOLKSWAGEN</t>
+  </si>
+  <si>
+    <t>GOLF</t>
+  </si>
+  <si>
+    <t>HATCHBACK 4 DOOR</t>
+  </si>
+  <si>
+    <t>8L V12</t>
+  </si>
+  <si>
+    <t>4WD</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>BACKDATED_SS_MAKE</t>
-  </si>
-  <si>
-    <t>7MSRP15H&amp;V</t>
-  </si>
-  <si>
-    <t>VOLKSWAGEN</t>
-  </si>
-  <si>
-    <t>GOLF</t>
-  </si>
-  <si>
-    <t>HATCHBACK 4 DOOR</t>
-  </si>
-  <si>
-    <t>8L V12</t>
-  </si>
-  <si>
-    <t>4WD</t>
-  </si>
-  <si>
-    <t>RT</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
 </sst>
 </file>
@@ -615,31 +615,31 @@
   <dimension ref="A1:AL3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
-    <col min="12" max="12" width="24.5546875" customWidth="1"/>
-    <col min="15" max="15" width="18.77734375" customWidth="1"/>
-    <col min="21" max="21" width="22.88671875" customWidth="1"/>
-    <col min="23" max="23" width="22.21875" customWidth="1"/>
-    <col min="24" max="24" width="20.88671875" customWidth="1"/>
-    <col min="25" max="25" width="34.77734375" customWidth="1"/>
-    <col min="26" max="26" width="5.88671875" customWidth="1"/>
-    <col min="27" max="27" width="16.21875" customWidth="1"/>
-    <col min="28" max="29" width="13.77734375" customWidth="1"/>
-    <col min="35" max="35" width="19.88671875" customWidth="1"/>
-    <col min="36" max="36" width="21.88671875" customWidth="1"/>
-    <col min="38" max="38" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="24.5703125" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" customWidth="1"/>
+    <col min="21" max="21" width="22.85546875" customWidth="1"/>
+    <col min="23" max="23" width="22.28515625" customWidth="1"/>
+    <col min="24" max="24" width="20.85546875" customWidth="1"/>
+    <col min="25" max="25" width="34.7109375" customWidth="1"/>
+    <col min="26" max="26" width="5.85546875" customWidth="1"/>
+    <col min="27" max="27" width="16.28515625" customWidth="1"/>
+    <col min="28" max="29" width="13.7109375" customWidth="1"/>
+    <col min="35" max="35" width="19.85546875" customWidth="1"/>
+    <col min="36" max="36" width="21.85546875" customWidth="1"/>
+    <col min="38" max="38" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -755,7 +755,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -766,10 +766,10 @@
         <v>2015</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" t="s">
-        <v>57</v>
+        <v>65</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="F2" t="s">
         <v>51</v>
@@ -871,9 +871,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>56</v>
@@ -882,16 +882,16 @@
         <v>2015</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="H3" s="3">
         <v>88888</v>
@@ -900,19 +900,19 @@
         <v>29</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O3" s="3">
         <v>12</v>
@@ -924,7 +924,7 @@
         <v>214</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S3" s="3">
         <v>4</v>
@@ -948,7 +948,7 @@
         <v>37</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AA3" s="3">
         <v>35</v>
@@ -963,16 +963,16 @@
         <v>39</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AG3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AH3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI3" s="3">
         <v>20000101</v>

</xml_diff>

<commit_message>
PAS-527: move back and forward classes and methods. Testdata changes.
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/backdatedVinTable_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/backdatedVinTable_UT_SS.xlsx
@@ -615,7 +615,7 @@
   <dimension ref="A1:AL3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D2" sqref="D2:AL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,7 +768,7 @@
       <c r="D2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F2" t="s">

</xml_diff>